<commit_message>
programmed and tested new search function queries.
</commit_message>
<xml_diff>
--- a/IEDC_Classification_fill/manual_insert/IEDC_95_CIRCOMOD_end_use_assets.xlsx
+++ b/IEDC_Classification_fill/manual_insert/IEDC_95_CIRCOMOD_end_use_assets.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAC518C-D276-447D-9D04-3CAF383E5474}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B8C5E-BC2A-4293-906E-B4768B977261}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,9 +356,6 @@
     <t>machinery and equipment</t>
   </si>
   <si>
-    <t>industrial machinergy and equipment</t>
-  </si>
-  <si>
     <t>energy supply assets</t>
   </si>
   <si>
@@ -434,9 +431,6 @@
     <t>energy infrastructure</t>
   </si>
   <si>
-    <t>other infrastructrure</t>
-  </si>
-  <si>
     <t>SNA 2008, 10.77</t>
   </si>
   <si>
@@ -492,13 +486,19 @@
   </si>
   <si>
     <t>CIRCOMOD project team</t>
+  </si>
+  <si>
+    <t>industrial machinery and equipment</t>
+  </si>
+  <si>
+    <t>other infrastructure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,13 +877,13 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18.83984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -903,16 +903,16 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -923,16 +923,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -941,7 +941,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -959,7 +959,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -968,7 +968,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -988,7 +988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -999,14 +999,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1039,14 +1039,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1079,74 +1079,74 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -1182,12 +1182,12 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1201,11 +1201,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.05078125" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.05078125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="3" width="8.578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
@@ -1215,7 +1215,7 @@
     <col min="11" max="11" width="19.62890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1317,13 +1317,13 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>67</v>
       </c>
       <c r="J3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K3" t="s">
         <v>96</v>
@@ -1332,7 +1332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1340,16 +1340,16 @@
         <v>95</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
         <v>96</v>
@@ -1358,7 +1358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1366,22 +1366,22 @@
         <v>95</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1389,19 +1389,19 @@
         <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1409,19 +1409,19 @@
         <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1429,19 +1429,19 @@
         <v>95</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1449,19 +1449,19 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1469,22 +1469,22 @@
         <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1492,22 +1492,22 @@
         <v>95</v>
       </c>
       <c r="D11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" t="s">
         <v>132</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>134</v>
-      </c>
       <c r="J11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1515,13 +1515,13 @@
         <v>95</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -1536,7 +1536,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1544,13 +1544,13 @@
         <v>95</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -1565,7 +1565,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>109</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>108</v>
@@ -1594,7 +1594,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1602,19 +1602,19 @@
         <v>95</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>80</v>
@@ -1623,7 +1623,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1631,23 +1631,23 @@
         <v>95</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>100</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K16" s="11" t="s">
         <v>80</v>
@@ -1656,7 +1656,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1664,10 +1664,10 @@
         <v>95</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>61</v>
@@ -1676,7 +1676,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>80</v>
@@ -1685,7 +1685,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1694,23 +1694,23 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1719,25 +1719,25 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1746,23 +1746,23 @@
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1770,19 +1770,19 @@
         <v>95</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="11" t="s">
         <v>80</v>
@@ -1791,7 +1791,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1799,19 +1799,19 @@
         <v>95</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K22" s="11" t="s">
         <v>80</v>
@@ -1820,7 +1820,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2028,37 +2028,37 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="6:10">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="6:10">
+    <row r="34" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J34" s="9"/>
     </row>
-    <row r="35" spans="6:10">
+    <row r="35" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J35" s="9"/>
     </row>
-    <row r="36" spans="6:10">
+    <row r="36" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J36" s="9"/>
     </row>
-    <row r="37" spans="6:10">
+    <row r="37" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="6:10">
+    <row r="38" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J38" s="9"/>
     </row>
-    <row r="39" spans="6:10">
+    <row r="39" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="6:10">
+    <row r="40" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="J40" s="9"/>
     </row>
-    <row r="41" spans="6:10">
+    <row r="41" spans="6:10" x14ac:dyDescent="0.55000000000000004">
       <c r="F41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="9"/>

</xml_diff>